<commit_message>
Added the rest of constraints section.
</commit_message>
<xml_diff>
--- a/Figures/Figures.xlsx
+++ b/Figures/Figures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nate/Documents/School/PhD/CS5113 COA/Project/Part1/gitProject/Block-Size-Optimization-for-VBASBS-Queueing-Model-for-Blockchain/Figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468C7A24-75A9-9044-97D1-48CC4C5E7B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC90D55-7780-804A-AFB1-7DF88A424128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{7561D3D1-DD51-0D46-B1F5-437A29696B28}"/>
   </bookViews>
@@ -6565,7 +6565,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>565150</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
@@ -6586,8 +6586,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000">
-          <a:off x="1397000" y="3543300"/>
-          <a:ext cx="317500" cy="330200"/>
+          <a:off x="1343025" y="3489325"/>
+          <a:ext cx="425450" cy="330200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7266,7 +7266,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>241300</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
@@ -7287,8 +7287,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000">
-          <a:off x="1860550" y="3130550"/>
-          <a:ext cx="317500" cy="330200"/>
+          <a:off x="1790700" y="3467100"/>
+          <a:ext cx="457200" cy="330200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7599,15 +7599,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>266701</xdr:colOff>
+      <xdr:colOff>309770</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>165101</xdr:rowOff>
+      <xdr:rowOff>48431</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>596901</xdr:colOff>
+      <xdr:colOff>639970</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>482601</xdr:rowOff>
+      <xdr:rowOff>498500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7622,8 +7622,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="18631428">
-          <a:off x="4400551" y="2228851"/>
-          <a:ext cx="317500" cy="330200"/>
+          <a:off x="4377335" y="2584866"/>
+          <a:ext cx="450069" cy="330200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11946,7 +11946,7 @@
   <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="65" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>